<commit_message>
create_contanct changes on 27/07/2023
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6A9E69FA-0793-4C6E-B4BA-E42DF470318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="DatProviderOrg" sheetId="3" r:id="rId2"/>
     <sheet name="Contact" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -104,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -519,10 +521,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -587,10 +589,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create Product commit on 21/08/2023
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6A9E69FA-0793-4C6E-B4BA-E42DF470318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026BACF-C2EE-4F7D-8D89-645E8A356962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="DatProviderOrg" sheetId="3" r:id="rId2"/>
     <sheet name="Contact" sheetId="2" r:id="rId3"/>
+    <sheet name="DatProviderProd" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>TC_ID</t>
   </si>
@@ -100,7 +100,25 @@
     <t>Electronics</t>
   </si>
   <si>
-    <t>xyz</t>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>CRM Applications</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Engineering</t>
   </si>
 </sst>
 </file>
@@ -165,13 +183,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +566,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -571,7 +590,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -579,7 +598,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -656,4 +675,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306037ED-59FB-4EDA-8A90-D9AAB7325E65}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
campainging Test case 25/08/23
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1026BACF-C2EE-4F7D-8D89-645E8A356962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364406C0-D9CC-4DA3-8A9F-D50A01303A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="DatProviderOrg" sheetId="3" r:id="rId2"/>
     <sheet name="Contact" sheetId="2" r:id="rId3"/>
     <sheet name="DatProviderProd" sheetId="4" r:id="rId4"/>
+    <sheet name="DatProviderCampaiging" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>TC_ID</t>
   </si>
@@ -119,6 +120,24 @@
   </si>
   <si>
     <t>Engineering</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>Trade Show</t>
+  </si>
+  <si>
+    <t>Public Relations</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Campaiging Name</t>
   </si>
 </sst>
 </file>
@@ -543,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -713,4 +732,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38FA203-487B-4E66-9B13-E54D0070FEE1}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #72 from Ansuman0/develop-branch"
This reverts commit 839c6be510fb7d38dd32c2bafab010a4cceba691, reversing
changes made to 255280b0defb1bf0278708eb047a297d9415187b.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3525E30B-C803-4225-B109-7E1A57AD62DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364406C0-D9CC-4DA3-8A9F-D50A01303A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="DatProviderOrg" sheetId="3" r:id="rId2"/>
-    <sheet name="DataProviderIndustryType" sheetId="7" r:id="rId3"/>
-    <sheet name="Contact" sheetId="2" r:id="rId4"/>
-    <sheet name="DatProviderProd" sheetId="4" r:id="rId5"/>
-    <sheet name="DatProviderCampaiging" sheetId="5" r:id="rId6"/>
-    <sheet name="DatProviderGlAccount" sheetId="6" r:id="rId7"/>
+    <sheet name="Contact" sheetId="2" r:id="rId3"/>
+    <sheet name="DatProviderProd" sheetId="4" r:id="rId4"/>
+    <sheet name="DatProviderCampaiging" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>TC_ID</t>
   </si>
@@ -141,36 +138,6 @@
   </si>
   <si>
     <t>Campaiging Name</t>
-  </si>
-  <si>
-    <t>GL Account</t>
-  </si>
-  <si>
-    <t>300-Sales-Software</t>
-  </si>
-  <si>
-    <t>301-Sales-Hardware</t>
-  </si>
-  <si>
-    <t>302-Rental-Income</t>
-  </si>
-  <si>
-    <t>303-Interest-Income</t>
-  </si>
-  <si>
-    <t>304-Sales-Software-Support</t>
-  </si>
-  <si>
-    <t>305-Sales Other</t>
-  </si>
-  <si>
-    <t>306-Internet Sales</t>
-  </si>
-  <si>
-    <t>307-Service-Hardware Labor</t>
-  </si>
-  <si>
-    <t>308-Sales-Books</t>
   </si>
 </sst>
 </file>
@@ -596,7 +563,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,54 +627,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B2024C-CA78-4617-A97D-1F1EB61D6A2E}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -777,7 +696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306037ED-59FB-4EDA-8A90-D9AAB7325E65}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -815,11 +734,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38FA203-487B-4E66-9B13-E54D0070FEE1}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -861,72 +780,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFE8457-AD91-4005-B64D-42E085ADF10D}">
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #72 from Ansuman0/develop-branch""
This reverts commit 34a3265d12098aaff447a7c965c1288319afaa74.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364406C0-D9CC-4DA3-8A9F-D50A01303A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3525E30B-C803-4225-B109-7E1A57AD62DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="DatProviderOrg" sheetId="3" r:id="rId2"/>
-    <sheet name="Contact" sheetId="2" r:id="rId3"/>
-    <sheet name="DatProviderProd" sheetId="4" r:id="rId4"/>
-    <sheet name="DatProviderCampaiging" sheetId="5" r:id="rId5"/>
+    <sheet name="DataProviderIndustryType" sheetId="7" r:id="rId3"/>
+    <sheet name="Contact" sheetId="2" r:id="rId4"/>
+    <sheet name="DatProviderProd" sheetId="4" r:id="rId5"/>
+    <sheet name="DatProviderCampaiging" sheetId="5" r:id="rId6"/>
+    <sheet name="DatProviderGlAccount" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:P11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>TC_ID</t>
   </si>
@@ -138,6 +141,36 @@
   </si>
   <si>
     <t>Campaiging Name</t>
+  </si>
+  <si>
+    <t>GL Account</t>
+  </si>
+  <si>
+    <t>300-Sales-Software</t>
+  </si>
+  <si>
+    <t>301-Sales-Hardware</t>
+  </si>
+  <si>
+    <t>302-Rental-Income</t>
+  </si>
+  <si>
+    <t>303-Interest-Income</t>
+  </si>
+  <si>
+    <t>304-Sales-Software-Support</t>
+  </si>
+  <si>
+    <t>305-Sales Other</t>
+  </si>
+  <si>
+    <t>306-Internet Sales</t>
+  </si>
+  <si>
+    <t>307-Service-Hardware Labor</t>
+  </si>
+  <si>
+    <t>308-Sales-Books</t>
   </si>
 </sst>
 </file>
@@ -563,7 +596,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,6 +660,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B2024C-CA78-4617-A97D-1F1EB61D6A2E}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -696,7 +777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306037ED-59FB-4EDA-8A90-D9AAB7325E65}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -734,11 +815,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38FA203-487B-4E66-9B13-E54D0070FEE1}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -780,4 +861,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFE8457-AD91-4005-B64D-42E085ADF10D}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>